<commit_message>
Added geonet/knet readers, wrote sm2xml and ftpfetch programs.
</commit_message>
<xml_diff>
--- a/tests/data/complete_pgm.xlsx
+++ b/tests/data/complete_pgm.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1600" yWindow="460" windowWidth="32040" windowHeight="21380"/>
+    <workbookView xWindow="1560" yWindow="460" windowWidth="32040" windowHeight="20540"/>
   </bookViews>
   <sheets>
     <sheet name="spectral_values.csv" sheetId="1" r:id="rId1"/>
@@ -81,12 +81,6 @@
     <t>location</t>
   </si>
   <si>
-    <t>latitude</t>
-  </si>
-  <si>
-    <t>longitude</t>
-  </si>
-  <si>
     <t>pga</t>
   </si>
   <si>
@@ -160,6 +154,12 @@
   </si>
   <si>
     <t>Mexican National Seismic Service report dated 2010-01-01</t>
+  </si>
+  <si>
+    <t>lat</t>
+  </si>
+  <si>
+    <t>lon</t>
   </si>
 </sst>
 </file>
@@ -624,7 +624,7 @@
   <dimension ref="A1:W21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -646,10 +646,10 @@
   <sheetData>
     <row r="1" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -660,39 +660,39 @@
         <v>19</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H2" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="10" t="s">
         <v>27</v>
-      </c>
-      <c r="I2" s="10" t="s">
-        <v>29</v>
       </c>
       <c r="J2" s="11"/>
       <c r="K2" s="11"/>
       <c r="L2" s="11"/>
       <c r="M2" s="12"/>
       <c r="N2" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="O2" s="11"/>
       <c r="P2" s="11"/>
       <c r="Q2" s="11"/>
       <c r="R2" s="12"/>
       <c r="S2" s="10" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="T2" s="11"/>
       <c r="U2" s="11"/>
@@ -701,49 +701,49 @@
     </row>
     <row r="3" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="I3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="L3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="M3" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="L3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>26</v>
-      </c>
       <c r="N3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="P3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="Q3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="P3" s="3" t="s">
+      <c r="R3" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="Q3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="R3" s="4" t="s">
-        <v>26</v>
-      </c>
       <c r="S3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="U3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="T3" s="3" t="s">
+      <c r="V3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="U3" s="3" t="s">
+      <c r="W3" s="4" t="s">
         <v>24</v>
-      </c>
-      <c r="V3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="W3" s="4" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -751,13 +751,13 @@
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E4" s="1">
         <v>20.043185999999999</v>
@@ -833,13 +833,13 @@
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E5" s="1">
         <v>16.874293999999999</v>
@@ -915,13 +915,13 @@
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E6" s="1">
         <v>17.213360999999999</v>
@@ -997,13 +997,13 @@
         <v>3</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E7" s="1">
         <v>16.247374000000001</v>
@@ -1078,13 +1078,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E8" s="1">
         <v>19.325265999999999</v>
@@ -1159,13 +1159,13 @@
         <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E9" s="1">
         <v>16.997788</v>
@@ -1241,13 +1241,13 @@
         <v>6</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E10" s="1">
         <v>17.798341000000001</v>
@@ -1323,13 +1323,13 @@
         <v>7</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E11" s="1">
         <v>16.565152999999999</v>
@@ -1405,13 +1405,13 @@
         <v>8</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E12" s="1">
         <v>17.067336999999998</v>
@@ -1487,13 +1487,13 @@
         <v>9</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E13" s="1">
         <v>17.065038999999999</v>
@@ -1569,13 +1569,13 @@
         <v>10</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E14" s="1">
         <v>15.666836999999999</v>
@@ -1651,13 +1651,13 @@
         <v>11</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E15" s="1">
         <v>17.535395999999999</v>
@@ -1733,13 +1733,13 @@
         <v>12</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E16" s="1">
         <v>19.044222999999999</v>
@@ -1815,13 +1815,13 @@
         <v>13</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E17" s="1">
         <v>18.904050999999999</v>
@@ -1897,13 +1897,13 @@
         <v>14</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E18" s="1">
         <v>17.98762</v>
@@ -1979,13 +1979,13 @@
         <v>15</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E19" s="1">
         <v>19.421758000000001</v>
@@ -2061,13 +2061,13 @@
         <v>16</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E20" s="1">
         <v>16.914259999999999</v>
@@ -2143,13 +2143,13 @@
         <v>17</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E21" s="1">
         <v>19.529875000000001</v>

</xml_diff>

<commit_message>
modified columns needed in dataframes, and also cleaned up name/location/loc issues in readers.
</commit_message>
<xml_diff>
--- a/tests/data/complete_pgm.xlsx
+++ b/tests/data/complete_pgm.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10319"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mhearne/src/python/shakemap-amp-tools/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{60CF62D2-B268-A64B-8D42-DEA60057D526}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="460" windowWidth="26200" windowHeight="13700"/>
+    <workbookView xWindow="1560" yWindow="460" windowWidth="26200" windowHeight="13700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="spectral_values.csv" sheetId="1" r:id="rId1"/>
@@ -78,9 +79,6 @@
     <t>station</t>
   </si>
   <si>
-    <t>location</t>
-  </si>
-  <si>
     <t>pga</t>
   </si>
   <si>
@@ -141,9 +139,6 @@
     <t>Veracruz</t>
   </si>
   <si>
-    <t>network</t>
-  </si>
-  <si>
     <t>source</t>
   </si>
   <si>
@@ -160,12 +155,18 @@
   </si>
   <si>
     <t>lon</t>
+  </si>
+  <si>
+    <t>netid</t>
+  </si>
+  <si>
+    <t>name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -617,14 +618,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:W21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -646,10 +647,10 @@
   <sheetData>
     <row r="1" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -657,42 +658,42 @@
         <v>18</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J2" s="11"/>
       <c r="K2" s="11"/>
       <c r="L2" s="11"/>
       <c r="M2" s="12"/>
       <c r="N2" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="O2" s="11"/>
       <c r="P2" s="11"/>
       <c r="Q2" s="11"/>
       <c r="R2" s="12"/>
       <c r="S2" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="T2" s="11"/>
       <c r="U2" s="11"/>
@@ -701,49 +702,49 @@
     </row>
     <row r="3" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="I3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="K3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="L3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="M3" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="M3" s="4" t="s">
-        <v>24</v>
-      </c>
       <c r="N3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="P3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="P3" s="3" t="s">
+      <c r="Q3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="Q3" s="3" t="s">
+      <c r="R3" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="R3" s="4" t="s">
-        <v>24</v>
-      </c>
       <c r="S3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="T3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="T3" s="3" t="s">
+      <c r="U3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="U3" s="3" t="s">
+      <c r="V3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="V3" s="3" t="s">
+      <c r="W3" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="W3" s="4" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -751,13 +752,13 @@
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E4" s="1">
         <v>20.043185999999999</v>
@@ -833,13 +834,13 @@
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E5" s="1">
         <v>16.874293999999999</v>
@@ -915,13 +916,13 @@
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E6" s="1">
         <v>17.213360999999999</v>
@@ -997,13 +998,13 @@
         <v>3</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E7" s="1">
         <v>16.247374000000001</v>
@@ -1078,13 +1079,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E8" s="1">
         <v>19.325265999999999</v>
@@ -1159,13 +1160,13 @@
         <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E9" s="1">
         <v>16.997788</v>
@@ -1241,13 +1242,13 @@
         <v>6</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E10" s="1">
         <v>17.798341000000001</v>
@@ -1323,13 +1324,13 @@
         <v>7</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E11" s="1">
         <v>16.565152999999999</v>
@@ -1405,13 +1406,13 @@
         <v>8</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E12" s="1">
         <v>17.067336999999998</v>
@@ -1487,13 +1488,13 @@
         <v>9</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E13" s="1">
         <v>17.065038999999999</v>
@@ -1569,13 +1570,13 @@
         <v>10</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E14" s="1">
         <v>15.666836999999999</v>
@@ -1651,13 +1652,13 @@
         <v>11</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E15" s="1">
         <v>17.535395999999999</v>
@@ -1733,13 +1734,13 @@
         <v>12</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E16" s="1">
         <v>19.044222999999999</v>
@@ -1815,13 +1816,13 @@
         <v>13</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E17" s="1">
         <v>18.904050999999999</v>
@@ -1897,13 +1898,13 @@
         <v>14</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E18" s="1">
         <v>17.98762</v>
@@ -1979,13 +1980,13 @@
         <v>15</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E19" s="1">
         <v>19.421758000000001</v>
@@ -2061,13 +2062,13 @@
         <v>16</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E20" s="1">
         <v>16.914259999999999</v>
@@ -2143,13 +2144,13 @@
         <v>17</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E21" s="1">
         <v>19.529875000000001</v>
@@ -2227,8 +2228,8 @@
     <mergeCell ref="S2:W2"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B19" r:id="rId1" tooltip="Michoacán" display="https://en.wikipedia.org/wiki/Michoac%C3%A1n"/>
-    <hyperlink ref="B21" r:id="rId2" tooltip="Veracruz" display="https://en.wikipedia.org/wiki/Veracruz"/>
+    <hyperlink ref="B19" r:id="rId1" tooltip="Michoacán" display="https://en.wikipedia.org/wiki/Michoac%C3%A1n" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B21" r:id="rId2" tooltip="Veracruz" display="https://en.wikipedia.org/wiki/Veracruz" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added elevation field to station, fixed flag to be a string not an int.
</commit_message>
<xml_diff>
--- a/tests/data/complete_pgm.xlsx
+++ b/tests/data/complete_pgm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mhearne/src/python/shakemap-amp-tools/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{60CF62D2-B268-A64B-8D42-DEA60057D526}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{E8DDEBD0-A1ED-1841-9F05-AFA218E421AD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="460" windowWidth="26200" windowHeight="13700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="48">
   <si>
     <t>ACAM</t>
   </si>
@@ -161,6 +161,9 @@
   </si>
   <si>
     <t>name</t>
+  </si>
+  <si>
+    <t>elev</t>
   </si>
 </sst>
 </file>
@@ -622,30 +625,30 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:W21"/>
+  <dimension ref="A1:X21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="8" max="8" width="7.5" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="6.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>41</v>
       </c>
@@ -653,7 +656,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>18</v>
       </c>
@@ -673,81 +676,84 @@
         <v>44</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="I2" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="J2" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="J2" s="11"/>
       <c r="K2" s="11"/>
       <c r="L2" s="11"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="10" t="s">
+      <c r="M2" s="11"/>
+      <c r="N2" s="12"/>
+      <c r="O2" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="O2" s="11"/>
       <c r="P2" s="11"/>
       <c r="Q2" s="11"/>
-      <c r="R2" s="12"/>
-      <c r="S2" s="10" t="s">
+      <c r="R2" s="11"/>
+      <c r="S2" s="12"/>
+      <c r="T2" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="T2" s="11"/>
       <c r="U2" s="11"/>
       <c r="V2" s="11"/>
-      <c r="W2" s="12"/>
+      <c r="W2" s="11"/>
+      <c r="X2" s="12"/>
     </row>
-    <row r="3" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="I3" s="2" t="s">
+    <row r="3" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="J3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="K3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="L3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="M3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="M3" s="4" t="s">
+      <c r="N3" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="O3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="P3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="P3" s="3" t="s">
+      <c r="Q3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="Q3" s="3" t="s">
+      <c r="R3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="R3" s="4" t="s">
+      <c r="S3" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="S3" s="2" t="s">
+      <c r="T3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="T3" s="3" t="s">
+      <c r="U3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="U3" s="3" t="s">
+      <c r="V3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="V3" s="3" t="s">
+      <c r="W3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="W3" s="4" t="s">
+      <c r="X3" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -767,69 +773,72 @@
         <v>-100.71677699999999</v>
       </c>
       <c r="G4" s="1">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="H4" s="1">
         <v>913.1</v>
       </c>
-      <c r="H4" s="8">
-        <f>3.66 *LOG10(I4) - 1.66</f>
+      <c r="I4" s="8">
+        <f>3.66 *LOG10(J4) - 1.66</f>
         <v>0.72367753123320733</v>
       </c>
-      <c r="I4" s="2">
+      <c r="J4" s="2">
         <v>4.4800000000000004</v>
       </c>
-      <c r="J4" s="3">
+      <c r="K4" s="3">
         <v>1.31</v>
       </c>
-      <c r="K4" s="3">
+      <c r="L4" s="3">
         <v>5.12</v>
       </c>
-      <c r="L4" s="3">
+      <c r="M4" s="3">
         <v>7.74</v>
       </c>
-      <c r="M4" s="4">
+      <c r="N4" s="4">
         <v>2.93</v>
       </c>
-      <c r="N4" s="2">
-        <f>I4*1.1</f>
+      <c r="O4" s="2">
+        <f>J4*1.1</f>
         <v>4.9280000000000008</v>
-      </c>
-      <c r="O4" s="3">
-        <f>J4*1.1</f>
-        <v>1.4410000000000003</v>
       </c>
       <c r="P4" s="3">
         <f>K4*1.1</f>
-        <v>5.6320000000000006</v>
+        <v>1.4410000000000003</v>
       </c>
       <c r="Q4" s="3">
         <f>L4*1.1</f>
+        <v>5.6320000000000006</v>
+      </c>
+      <c r="R4" s="3">
+        <f>M4*1.1</f>
         <v>8.5140000000000011</v>
       </c>
-      <c r="R4" s="4">
-        <f>M4*1.1</f>
+      <c r="S4" s="4">
+        <f>N4*1.1</f>
         <v>3.2230000000000003</v>
       </c>
-      <c r="S4" s="2">
-        <f>I4*0.95</f>
+      <c r="T4" s="2">
+        <f>J4*0.95</f>
         <v>4.2560000000000002</v>
       </c>
-      <c r="T4" s="2">
-        <f t="shared" ref="T4:W4" si="0">J4*0.95</f>
+      <c r="U4" s="2">
+        <f t="shared" ref="U4:X4" si="0">K4*0.95</f>
         <v>1.2444999999999999</v>
       </c>
-      <c r="U4" s="2">
+      <c r="V4" s="2">
         <f t="shared" si="0"/>
         <v>4.8639999999999999</v>
       </c>
-      <c r="V4" s="2">
+      <c r="W4" s="2">
         <f t="shared" si="0"/>
         <v>7.3529999999999998</v>
       </c>
-      <c r="W4" s="2">
+      <c r="X4" s="2">
         <f t="shared" si="0"/>
         <v>2.7835000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
@@ -849,69 +858,72 @@
         <v>-99.886505</v>
       </c>
       <c r="G5" s="1">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="H5" s="1">
         <v>672.4</v>
       </c>
-      <c r="H5" s="8">
-        <f>3.66 *LOG10(I5) - 1.66</f>
+      <c r="I5" s="8">
+        <f>3.66 *LOG10(J5) - 1.66</f>
         <v>4.0075548582081897</v>
       </c>
-      <c r="I5" s="2">
+      <c r="J5" s="2">
         <v>35.36</v>
       </c>
-      <c r="J5" s="3">
+      <c r="K5" s="3">
         <v>1.35</v>
       </c>
-      <c r="K5" s="3">
+      <c r="L5" s="3">
         <v>73.08</v>
       </c>
-      <c r="L5" s="3">
+      <c r="M5" s="3">
         <v>7.36</v>
       </c>
-      <c r="M5" s="4">
+      <c r="N5" s="4">
         <v>1.88</v>
       </c>
-      <c r="N5" s="2">
-        <f t="shared" ref="N5:N21" si="1">I5*1.1</f>
+      <c r="O5" s="2">
+        <f t="shared" ref="O5:O21" si="1">J5*1.1</f>
         <v>38.896000000000001</v>
       </c>
-      <c r="O5" s="3">
-        <f t="shared" ref="O5:O21" si="2">J5*1.1</f>
+      <c r="P5" s="3">
+        <f t="shared" ref="P5:P21" si="2">K5*1.1</f>
         <v>1.4850000000000003</v>
       </c>
-      <c r="P5" s="3">
-        <f t="shared" ref="P5:P21" si="3">K5*1.1</f>
+      <c r="Q5" s="3">
+        <f t="shared" ref="Q5:Q21" si="3">L5*1.1</f>
         <v>80.388000000000005</v>
       </c>
-      <c r="Q5" s="3">
-        <f t="shared" ref="Q5:Q21" si="4">L5*1.1</f>
+      <c r="R5" s="3">
+        <f t="shared" ref="R5:R21" si="4">M5*1.1</f>
         <v>8.0960000000000019</v>
       </c>
-      <c r="R5" s="4">
-        <f t="shared" ref="R5:R21" si="5">M5*1.1</f>
+      <c r="S5" s="4">
+        <f t="shared" ref="S5:S21" si="5">N5*1.1</f>
         <v>2.0680000000000001</v>
       </c>
-      <c r="S5" s="2">
-        <f t="shared" ref="S5:S21" si="6">I5*0.95</f>
+      <c r="T5" s="2">
+        <f t="shared" ref="T5:T21" si="6">J5*0.95</f>
         <v>33.591999999999999</v>
       </c>
-      <c r="T5" s="2">
-        <f t="shared" ref="T5:T21" si="7">J5*0.95</f>
+      <c r="U5" s="2">
+        <f t="shared" ref="U5:U21" si="7">K5*0.95</f>
         <v>1.2825</v>
       </c>
-      <c r="U5" s="2">
-        <f t="shared" ref="U5:U21" si="8">K5*0.95</f>
+      <c r="V5" s="2">
+        <f t="shared" ref="V5:V21" si="8">L5*0.95</f>
         <v>69.426000000000002</v>
       </c>
-      <c r="V5" s="2">
-        <f t="shared" ref="V5:V21" si="9">L5*0.95</f>
+      <c r="W5" s="2">
+        <f t="shared" ref="W5:W21" si="9">M5*0.95</f>
         <v>6.992</v>
       </c>
-      <c r="W5" s="2">
-        <f t="shared" ref="W5:W21" si="10">M5*0.95</f>
+      <c r="X5" s="2">
+        <f t="shared" ref="X5:X21" si="10">N5*0.95</f>
         <v>1.7859999999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
@@ -931,69 +943,72 @@
         <v>-100.43226900000001</v>
       </c>
       <c r="G6" s="1">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="H6" s="1">
         <v>739.1</v>
       </c>
-      <c r="H6" s="8">
-        <f>3.66 *LOG10(I6) - 1.66</f>
+      <c r="I6" s="8">
+        <f>3.66 *LOG10(J6) - 1.66</f>
         <v>2.9940900430465254</v>
       </c>
-      <c r="I6" s="2">
+      <c r="J6" s="2">
         <v>18.690000000000001</v>
       </c>
-      <c r="J6" s="3">
+      <c r="K6" s="3">
         <v>0.67</v>
       </c>
-      <c r="K6" s="3">
+      <c r="L6" s="3">
         <v>25.45</v>
       </c>
-      <c r="L6" s="3">
+      <c r="M6" s="3">
         <v>8.1999999999999993</v>
       </c>
-      <c r="M6" s="4">
+      <c r="N6" s="4">
         <v>3.09</v>
       </c>
-      <c r="N6" s="2">
+      <c r="O6" s="2">
         <f t="shared" si="1"/>
         <v>20.559000000000005</v>
       </c>
-      <c r="O6" s="3">
+      <c r="P6" s="3">
         <f t="shared" si="2"/>
         <v>0.7370000000000001</v>
       </c>
-      <c r="P6" s="3">
+      <c r="Q6" s="3">
         <f t="shared" si="3"/>
         <v>27.995000000000001</v>
       </c>
-      <c r="Q6" s="3">
+      <c r="R6" s="3">
         <f t="shared" si="4"/>
         <v>9.02</v>
       </c>
-      <c r="R6" s="4">
+      <c r="S6" s="4">
         <f t="shared" si="5"/>
         <v>3.399</v>
       </c>
-      <c r="S6" s="2">
+      <c r="T6" s="2">
         <f t="shared" si="6"/>
         <v>17.755500000000001</v>
       </c>
-      <c r="T6" s="2">
+      <c r="U6" s="2">
         <f t="shared" si="7"/>
         <v>0.63649999999999995</v>
       </c>
-      <c r="U6" s="2">
+      <c r="V6" s="2">
         <f t="shared" si="8"/>
         <v>24.177499999999998</v>
       </c>
-      <c r="V6" s="2">
+      <c r="W6" s="2">
         <f t="shared" si="9"/>
         <v>7.7899999999999991</v>
       </c>
-      <c r="W6" s="2">
+      <c r="X6" s="2">
         <f t="shared" si="10"/>
         <v>2.9354999999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
@@ -1013,68 +1028,71 @@
         <v>-93.912575000000004</v>
       </c>
       <c r="G7" s="1">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="H7" s="1">
         <v>136.30000000000001</v>
       </c>
-      <c r="H7" s="8">
+      <c r="I7" s="8">
         <v>0</v>
       </c>
-      <c r="I7" s="2">
+      <c r="J7" s="2">
         <v>2.16</v>
       </c>
-      <c r="J7" s="3">
+      <c r="K7" s="3">
         <v>0.27</v>
       </c>
-      <c r="K7" s="3">
+      <c r="L7" s="3">
         <v>3.41</v>
       </c>
-      <c r="L7" s="3">
+      <c r="M7" s="3">
         <v>2.34</v>
       </c>
-      <c r="M7" s="4">
+      <c r="N7" s="4">
         <v>0.95</v>
       </c>
-      <c r="N7" s="2">
+      <c r="O7" s="2">
         <f t="shared" si="1"/>
         <v>2.3760000000000003</v>
       </c>
-      <c r="O7" s="3">
+      <c r="P7" s="3">
         <f t="shared" si="2"/>
         <v>0.29700000000000004</v>
       </c>
-      <c r="P7" s="3">
+      <c r="Q7" s="3">
         <f t="shared" si="3"/>
         <v>3.7510000000000003</v>
       </c>
-      <c r="Q7" s="3">
+      <c r="R7" s="3">
         <f t="shared" si="4"/>
         <v>2.5739999999999998</v>
       </c>
-      <c r="R7" s="4">
+      <c r="S7" s="4">
         <f t="shared" si="5"/>
         <v>1.0449999999999999</v>
       </c>
-      <c r="S7" s="2">
+      <c r="T7" s="2">
         <f t="shared" si="6"/>
         <v>2.052</v>
       </c>
-      <c r="T7" s="2">
+      <c r="U7" s="2">
         <f t="shared" si="7"/>
         <v>0.25650000000000001</v>
       </c>
-      <c r="U7" s="2">
+      <c r="V7" s="2">
         <f t="shared" si="8"/>
         <v>3.2395</v>
       </c>
-      <c r="V7" s="2">
+      <c r="W7" s="2">
         <f t="shared" si="9"/>
         <v>2.2229999999999999</v>
       </c>
-      <c r="W7" s="2">
+      <c r="X7" s="2">
         <f t="shared" si="10"/>
         <v>0.90249999999999997</v>
       </c>
     </row>
-    <row r="8" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
@@ -1094,68 +1112,71 @@
         <v>-103.760813</v>
       </c>
       <c r="G8" s="1">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="H8" s="1">
         <v>1151</v>
       </c>
-      <c r="H8" s="8">
+      <c r="I8" s="8">
         <v>0</v>
       </c>
-      <c r="I8" s="2">
+      <c r="J8" s="2">
         <v>2.23</v>
       </c>
-      <c r="J8" s="3">
+      <c r="K8" s="3">
         <v>0.44</v>
       </c>
-      <c r="K8" s="3">
+      <c r="L8" s="3">
         <v>5.42</v>
       </c>
-      <c r="L8" s="3">
+      <c r="M8" s="3">
         <v>7.7</v>
       </c>
-      <c r="M8" s="4">
+      <c r="N8" s="4">
         <v>2.2200000000000002</v>
       </c>
-      <c r="N8" s="2">
+      <c r="O8" s="2">
         <f t="shared" si="1"/>
         <v>2.4530000000000003</v>
       </c>
-      <c r="O8" s="3">
+      <c r="P8" s="3">
         <f t="shared" si="2"/>
         <v>0.48400000000000004</v>
       </c>
-      <c r="P8" s="3">
+      <c r="Q8" s="3">
         <f t="shared" si="3"/>
         <v>5.9620000000000006</v>
       </c>
-      <c r="Q8" s="3">
+      <c r="R8" s="3">
         <f t="shared" si="4"/>
         <v>8.4700000000000006</v>
       </c>
-      <c r="R8" s="4">
+      <c r="S8" s="4">
         <f t="shared" si="5"/>
         <v>2.4420000000000006</v>
       </c>
-      <c r="S8" s="2">
+      <c r="T8" s="2">
         <f t="shared" si="6"/>
         <v>2.1185</v>
       </c>
-      <c r="T8" s="2">
+      <c r="U8" s="2">
         <f t="shared" si="7"/>
         <v>0.41799999999999998</v>
       </c>
-      <c r="U8" s="2">
+      <c r="V8" s="2">
         <f t="shared" si="8"/>
         <v>5.149</v>
       </c>
-      <c r="V8" s="2">
+      <c r="W8" s="2">
         <f t="shared" si="9"/>
         <v>7.3149999999999995</v>
       </c>
-      <c r="W8" s="2">
+      <c r="X8" s="2">
         <f t="shared" si="10"/>
         <v>2.109</v>
       </c>
     </row>
-    <row r="9" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
@@ -1175,69 +1196,72 @@
         <v>-100.089963</v>
       </c>
       <c r="G9" s="1">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="H9" s="1">
         <v>697.2</v>
       </c>
-      <c r="H9" s="8">
-        <f t="shared" ref="H9:H21" si="11">3.66 *LOG10(I9) - 1.66</f>
+      <c r="I9" s="8">
+        <f t="shared" ref="I9:I21" si="11">3.66 *LOG10(J9) - 1.66</f>
         <v>2.9623072177545042</v>
       </c>
-      <c r="I9" s="2">
+      <c r="J9" s="2">
         <v>18.32</v>
       </c>
-      <c r="J9" s="3">
+      <c r="K9" s="3">
         <v>0.86</v>
       </c>
-      <c r="K9" s="3">
+      <c r="L9" s="3">
         <v>19.97</v>
       </c>
-      <c r="L9" s="3">
+      <c r="M9" s="3">
         <v>8.16</v>
       </c>
-      <c r="M9" s="4">
+      <c r="N9" s="4">
         <v>1.73</v>
       </c>
-      <c r="N9" s="2">
+      <c r="O9" s="2">
         <f t="shared" si="1"/>
         <v>20.152000000000001</v>
       </c>
-      <c r="O9" s="3">
+      <c r="P9" s="3">
         <f t="shared" si="2"/>
         <v>0.94600000000000006</v>
       </c>
-      <c r="P9" s="3">
+      <c r="Q9" s="3">
         <f t="shared" si="3"/>
         <v>21.966999999999999</v>
       </c>
-      <c r="Q9" s="3">
+      <c r="R9" s="3">
         <f t="shared" si="4"/>
         <v>8.9760000000000009</v>
       </c>
-      <c r="R9" s="4">
+      <c r="S9" s="4">
         <f t="shared" si="5"/>
         <v>1.903</v>
       </c>
-      <c r="S9" s="2">
+      <c r="T9" s="2">
         <f t="shared" si="6"/>
         <v>17.404</v>
       </c>
-      <c r="T9" s="2">
+      <c r="U9" s="2">
         <f t="shared" si="7"/>
         <v>0.81699999999999995</v>
       </c>
-      <c r="U9" s="2">
+      <c r="V9" s="2">
         <f t="shared" si="8"/>
         <v>18.971499999999999</v>
       </c>
-      <c r="V9" s="2">
+      <c r="W9" s="2">
         <f t="shared" si="9"/>
         <v>7.7519999999999998</v>
       </c>
-      <c r="W9" s="2">
+      <c r="X9" s="2">
         <f t="shared" si="10"/>
         <v>1.6435</v>
       </c>
     </row>
-    <row r="10" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
@@ -1257,69 +1281,72 @@
         <v>-98.559717000000006</v>
       </c>
       <c r="G10" s="1">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="H10" s="1">
         <v>585.1</v>
       </c>
-      <c r="H10" s="8">
+      <c r="I10" s="8">
         <f t="shared" si="11"/>
         <v>6.5085773089009038</v>
       </c>
-      <c r="I10" s="2">
+      <c r="J10" s="2">
         <v>170.55</v>
       </c>
-      <c r="J10" s="3">
+      <c r="K10" s="3">
         <v>12.1</v>
       </c>
-      <c r="K10" s="3">
+      <c r="L10" s="3">
         <v>332.21</v>
       </c>
-      <c r="L10" s="3">
+      <c r="M10" s="3">
         <v>69.61</v>
       </c>
-      <c r="M10" s="4">
+      <c r="N10" s="4">
         <v>21.7</v>
       </c>
-      <c r="N10" s="2">
+      <c r="O10" s="2">
         <f t="shared" si="1"/>
         <v>187.60500000000002</v>
       </c>
-      <c r="O10" s="3">
+      <c r="P10" s="3">
         <f t="shared" si="2"/>
         <v>13.31</v>
       </c>
-      <c r="P10" s="3">
+      <c r="Q10" s="3">
         <f t="shared" si="3"/>
         <v>365.43099999999998</v>
       </c>
-      <c r="Q10" s="3">
+      <c r="R10" s="3">
         <f t="shared" si="4"/>
         <v>76.571000000000012</v>
       </c>
-      <c r="R10" s="4">
+      <c r="S10" s="4">
         <f t="shared" si="5"/>
         <v>23.87</v>
       </c>
-      <c r="S10" s="2">
+      <c r="T10" s="2">
         <f t="shared" si="6"/>
         <v>162.02250000000001</v>
       </c>
-      <c r="T10" s="2">
+      <c r="U10" s="2">
         <f t="shared" si="7"/>
         <v>11.494999999999999</v>
       </c>
-      <c r="U10" s="2">
+      <c r="V10" s="2">
         <f t="shared" si="8"/>
         <v>315.59949999999998</v>
       </c>
-      <c r="V10" s="2">
+      <c r="W10" s="2">
         <f t="shared" si="9"/>
         <v>66.129499999999993</v>
       </c>
-      <c r="W10" s="2">
+      <c r="X10" s="2">
         <f t="shared" si="10"/>
         <v>20.614999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
@@ -1339,69 +1366,72 @@
         <v>-94.616946999999996</v>
       </c>
       <c r="G11" s="1">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="H11" s="1">
         <v>188</v>
       </c>
-      <c r="H11" s="8">
+      <c r="I11" s="8">
         <f t="shared" si="11"/>
         <v>1.1827263333975842</v>
       </c>
-      <c r="I11" s="2">
+      <c r="J11" s="2">
         <v>5.98</v>
       </c>
-      <c r="J11" s="3">
+      <c r="K11" s="3">
         <v>0.28999999999999998</v>
       </c>
-      <c r="K11" s="3">
+      <c r="L11" s="3">
         <v>6.4</v>
       </c>
-      <c r="L11" s="3">
+      <c r="M11" s="3">
         <v>3.81</v>
       </c>
-      <c r="M11" s="4">
+      <c r="N11" s="4">
         <v>1.1100000000000001</v>
       </c>
-      <c r="N11" s="2">
+      <c r="O11" s="2">
         <f t="shared" si="1"/>
         <v>6.5780000000000012</v>
       </c>
-      <c r="O11" s="3">
+      <c r="P11" s="3">
         <f t="shared" si="2"/>
         <v>0.31900000000000001</v>
       </c>
-      <c r="P11" s="3">
+      <c r="Q11" s="3">
         <f t="shared" si="3"/>
         <v>7.0400000000000009</v>
       </c>
-      <c r="Q11" s="3">
+      <c r="R11" s="3">
         <f t="shared" si="4"/>
         <v>4.1910000000000007</v>
       </c>
-      <c r="R11" s="4">
+      <c r="S11" s="4">
         <f t="shared" si="5"/>
         <v>1.2210000000000003</v>
       </c>
-      <c r="S11" s="2">
+      <c r="T11" s="2">
         <f t="shared" si="6"/>
         <v>5.681</v>
       </c>
-      <c r="T11" s="2">
+      <c r="U11" s="2">
         <f t="shared" si="7"/>
         <v>0.27549999999999997</v>
       </c>
-      <c r="U11" s="2">
+      <c r="V11" s="2">
         <f t="shared" si="8"/>
         <v>6.08</v>
       </c>
-      <c r="V11" s="2">
+      <c r="W11" s="2">
         <f t="shared" si="9"/>
         <v>3.6194999999999999</v>
       </c>
-      <c r="W11" s="2">
+      <c r="X11" s="2">
         <f t="shared" si="10"/>
         <v>1.0545</v>
       </c>
     </row>
-    <row r="12" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
@@ -1421,69 +1451,72 @@
         <v>-96.723804000000001</v>
       </c>
       <c r="G12" s="1">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="H12" s="1">
         <v>377.9</v>
       </c>
-      <c r="H12" s="8">
+      <c r="I12" s="8">
         <f t="shared" si="11"/>
         <v>2.9439815281494539</v>
       </c>
-      <c r="I12" s="2">
+      <c r="J12" s="2">
         <v>18.11</v>
       </c>
-      <c r="J12" s="3">
+      <c r="K12" s="3">
         <v>1.45</v>
       </c>
-      <c r="K12" s="3">
+      <c r="L12" s="3">
         <v>52.5</v>
       </c>
-      <c r="L12" s="3">
+      <c r="M12" s="3">
         <v>20.04</v>
       </c>
-      <c r="M12" s="4">
+      <c r="N12" s="4">
         <v>3.13</v>
       </c>
-      <c r="N12" s="2">
+      <c r="O12" s="2">
         <f t="shared" si="1"/>
         <v>19.920999999999999</v>
       </c>
-      <c r="O12" s="3">
+      <c r="P12" s="3">
         <f t="shared" si="2"/>
         <v>1.595</v>
       </c>
-      <c r="P12" s="3">
+      <c r="Q12" s="3">
         <f t="shared" si="3"/>
         <v>57.750000000000007</v>
       </c>
-      <c r="Q12" s="3">
+      <c r="R12" s="3">
         <f t="shared" si="4"/>
         <v>22.044</v>
       </c>
-      <c r="R12" s="4">
+      <c r="S12" s="4">
         <f t="shared" si="5"/>
         <v>3.4430000000000001</v>
       </c>
-      <c r="S12" s="2">
+      <c r="T12" s="2">
         <f t="shared" si="6"/>
         <v>17.204499999999999</v>
       </c>
-      <c r="T12" s="2">
+      <c r="U12" s="2">
         <f t="shared" si="7"/>
         <v>1.3774999999999999</v>
       </c>
-      <c r="U12" s="2">
+      <c r="V12" s="2">
         <f t="shared" si="8"/>
         <v>49.875</v>
       </c>
-      <c r="V12" s="2">
+      <c r="W12" s="2">
         <f t="shared" si="9"/>
         <v>19.037999999999997</v>
       </c>
-      <c r="W12" s="2">
+      <c r="X12" s="2">
         <f t="shared" si="10"/>
         <v>2.9734999999999996</v>
       </c>
     </row>
-    <row r="13" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
@@ -1503,69 +1536,72 @@
         <v>-96.703157000000004</v>
       </c>
       <c r="G13" s="1">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="H13" s="1">
         <v>376</v>
       </c>
-      <c r="H13" s="8">
+      <c r="I13" s="8">
         <f t="shared" si="11"/>
         <v>3.2904002934162691</v>
       </c>
-      <c r="I13" s="2">
+      <c r="J13" s="2">
         <v>22.52</v>
       </c>
-      <c r="J13" s="3">
+      <c r="K13" s="3">
         <v>1.34</v>
       </c>
-      <c r="K13" s="3">
+      <c r="L13" s="3">
         <v>81.95</v>
       </c>
-      <c r="L13" s="3">
+      <c r="M13" s="3">
         <v>34.270000000000003</v>
       </c>
-      <c r="M13" s="4">
+      <c r="N13" s="4">
         <v>3.8</v>
       </c>
-      <c r="N13" s="2">
+      <c r="O13" s="2">
         <f t="shared" si="1"/>
         <v>24.772000000000002</v>
       </c>
-      <c r="O13" s="3">
+      <c r="P13" s="3">
         <f t="shared" si="2"/>
         <v>1.4740000000000002</v>
       </c>
-      <c r="P13" s="3">
+      <c r="Q13" s="3">
         <f t="shared" si="3"/>
         <v>90.14500000000001</v>
       </c>
-      <c r="Q13" s="3">
+      <c r="R13" s="3">
         <f t="shared" si="4"/>
         <v>37.69700000000001</v>
       </c>
-      <c r="R13" s="4">
+      <c r="S13" s="4">
         <f t="shared" si="5"/>
         <v>4.18</v>
       </c>
-      <c r="S13" s="2">
+      <c r="T13" s="2">
         <f t="shared" si="6"/>
         <v>21.393999999999998</v>
       </c>
-      <c r="T13" s="2">
+      <c r="U13" s="2">
         <f t="shared" si="7"/>
         <v>1.2729999999999999</v>
       </c>
-      <c r="U13" s="2">
+      <c r="V13" s="2">
         <f t="shared" si="8"/>
         <v>77.852499999999992</v>
       </c>
-      <c r="V13" s="2">
+      <c r="W13" s="2">
         <f t="shared" si="9"/>
         <v>32.5565</v>
       </c>
-      <c r="W13" s="2">
+      <c r="X13" s="2">
         <f t="shared" si="10"/>
         <v>3.61</v>
       </c>
     </row>
-    <row r="14" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
@@ -1585,69 +1621,72 @@
         <v>-96.490505999999996</v>
       </c>
       <c r="G14" s="1">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="H14" s="1">
         <v>287</v>
       </c>
-      <c r="H14" s="8">
+      <c r="I14" s="8">
         <f t="shared" si="11"/>
         <v>0.79309982225129416</v>
       </c>
-      <c r="I14" s="2">
+      <c r="J14" s="2">
         <v>4.68</v>
       </c>
-      <c r="J14" s="3">
+      <c r="K14" s="3">
         <v>0.51</v>
       </c>
-      <c r="K14" s="3">
+      <c r="L14" s="3">
         <v>5.77</v>
       </c>
-      <c r="L14" s="3">
+      <c r="M14" s="3">
         <v>4.95</v>
       </c>
-      <c r="M14" s="4">
+      <c r="N14" s="4">
         <v>1.65</v>
       </c>
-      <c r="N14" s="2">
+      <c r="O14" s="2">
         <f t="shared" si="1"/>
         <v>5.1479999999999997</v>
       </c>
-      <c r="O14" s="3">
+      <c r="P14" s="3">
         <f t="shared" si="2"/>
         <v>0.56100000000000005</v>
       </c>
-      <c r="P14" s="3">
+      <c r="Q14" s="3">
         <f t="shared" si="3"/>
         <v>6.3470000000000004</v>
       </c>
-      <c r="Q14" s="3">
+      <c r="R14" s="3">
         <f t="shared" si="4"/>
         <v>5.4450000000000003</v>
       </c>
-      <c r="R14" s="4">
+      <c r="S14" s="4">
         <f t="shared" si="5"/>
         <v>1.8149999999999999</v>
       </c>
-      <c r="S14" s="2">
+      <c r="T14" s="2">
         <f t="shared" si="6"/>
         <v>4.4459999999999997</v>
       </c>
-      <c r="T14" s="2">
+      <c r="U14" s="2">
         <f t="shared" si="7"/>
         <v>0.48449999999999999</v>
       </c>
-      <c r="U14" s="2">
+      <c r="V14" s="2">
         <f t="shared" si="8"/>
         <v>5.4814999999999996</v>
       </c>
-      <c r="V14" s="2">
+      <c r="W14" s="2">
         <f t="shared" si="9"/>
         <v>4.7024999999999997</v>
       </c>
-      <c r="W14" s="2">
+      <c r="X14" s="2">
         <f t="shared" si="10"/>
         <v>1.5674999999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>11</v>
       </c>
@@ -1667,69 +1706,72 @@
         <v>-101.262608</v>
       </c>
       <c r="G15" s="1">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="H15" s="1">
         <v>834.1</v>
       </c>
-      <c r="H15" s="8">
+      <c r="I15" s="8">
         <f t="shared" si="11"/>
         <v>2.0047614148547304</v>
       </c>
-      <c r="I15" s="2">
+      <c r="J15" s="2">
         <v>10.029999999999999</v>
       </c>
-      <c r="J15" s="3">
+      <c r="K15" s="3">
         <v>0.44</v>
       </c>
-      <c r="K15" s="3">
+      <c r="L15" s="3">
         <v>20.7</v>
       </c>
-      <c r="L15" s="3">
+      <c r="M15" s="3">
         <v>6.05</v>
       </c>
-      <c r="M15" s="4">
+      <c r="N15" s="4">
         <v>2.0499999999999998</v>
       </c>
-      <c r="N15" s="2">
+      <c r="O15" s="2">
         <f t="shared" si="1"/>
         <v>11.032999999999999</v>
       </c>
-      <c r="O15" s="3">
+      <c r="P15" s="3">
         <f t="shared" si="2"/>
         <v>0.48400000000000004</v>
       </c>
-      <c r="P15" s="3">
+      <c r="Q15" s="3">
         <f t="shared" si="3"/>
         <v>22.77</v>
       </c>
-      <c r="Q15" s="3">
+      <c r="R15" s="3">
         <f t="shared" si="4"/>
         <v>6.6550000000000002</v>
       </c>
-      <c r="R15" s="4">
+      <c r="S15" s="4">
         <f t="shared" si="5"/>
         <v>2.2549999999999999</v>
       </c>
-      <c r="S15" s="2">
+      <c r="T15" s="2">
         <f t="shared" si="6"/>
         <v>9.5284999999999993</v>
       </c>
-      <c r="T15" s="2">
+      <c r="U15" s="2">
         <f t="shared" si="7"/>
         <v>0.41799999999999998</v>
       </c>
-      <c r="U15" s="2">
+      <c r="V15" s="2">
         <f t="shared" si="8"/>
         <v>19.664999999999999</v>
       </c>
-      <c r="V15" s="2">
+      <c r="W15" s="2">
         <f t="shared" si="9"/>
         <v>5.7474999999999996</v>
       </c>
-      <c r="W15" s="2">
+      <c r="X15" s="2">
         <f t="shared" si="10"/>
         <v>1.9474999999999998</v>
       </c>
     </row>
-    <row r="16" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
@@ -1749,69 +1791,72 @@
         <v>-98.168465999999995</v>
       </c>
       <c r="G16" s="1">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="H16" s="1">
         <v>637.1</v>
       </c>
-      <c r="H16" s="8">
+      <c r="I16" s="8">
         <f t="shared" si="11"/>
         <v>6.2143501408750526</v>
       </c>
-      <c r="I16" s="2">
+      <c r="J16" s="2">
         <v>141.72999999999999</v>
       </c>
-      <c r="J16" s="3">
+      <c r="K16" s="3">
         <v>9.84</v>
       </c>
-      <c r="K16" s="3">
+      <c r="L16" s="3">
         <v>308.33999999999997</v>
       </c>
-      <c r="L16" s="3">
+      <c r="M16" s="3">
         <v>97.32</v>
       </c>
-      <c r="M16" s="4">
+      <c r="N16" s="4">
         <v>24.13</v>
       </c>
-      <c r="N16" s="2">
+      <c r="O16" s="2">
         <f t="shared" si="1"/>
         <v>155.90299999999999</v>
       </c>
-      <c r="O16" s="3">
+      <c r="P16" s="3">
         <f t="shared" si="2"/>
         <v>10.824</v>
       </c>
-      <c r="P16" s="3">
+      <c r="Q16" s="3">
         <f t="shared" si="3"/>
         <v>339.17399999999998</v>
       </c>
-      <c r="Q16" s="3">
+      <c r="R16" s="3">
         <f t="shared" si="4"/>
         <v>107.05200000000001</v>
       </c>
-      <c r="R16" s="4">
+      <c r="S16" s="4">
         <f t="shared" si="5"/>
         <v>26.543000000000003</v>
       </c>
-      <c r="S16" s="2">
+      <c r="T16" s="2">
         <f t="shared" si="6"/>
         <v>134.64349999999999</v>
       </c>
-      <c r="T16" s="2">
+      <c r="U16" s="2">
         <f t="shared" si="7"/>
         <v>9.347999999999999</v>
       </c>
-      <c r="U16" s="2">
+      <c r="V16" s="2">
         <f t="shared" si="8"/>
         <v>292.92299999999994</v>
       </c>
-      <c r="V16" s="2">
+      <c r="W16" s="2">
         <f t="shared" si="9"/>
         <v>92.453999999999994</v>
       </c>
-      <c r="W16" s="2">
+      <c r="X16" s="2">
         <f t="shared" si="10"/>
         <v>22.923499999999997</v>
       </c>
     </row>
-    <row r="17" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
@@ -1831,69 +1876,72 @@
         <v>-100.159615</v>
       </c>
       <c r="G17" s="1">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="H17" s="1">
         <v>793.4</v>
       </c>
-      <c r="H17" s="8">
+      <c r="I17" s="8">
         <f t="shared" si="11"/>
         <v>5.3695607051488423</v>
       </c>
-      <c r="I17" s="2">
+      <c r="J17" s="2">
         <v>83.3</v>
       </c>
-      <c r="J17" s="3">
+      <c r="K17" s="3">
         <v>3.53</v>
       </c>
-      <c r="K17" s="3">
+      <c r="L17" s="3">
         <v>120.14</v>
       </c>
-      <c r="L17" s="3">
+      <c r="M17" s="3">
         <v>42.08</v>
       </c>
-      <c r="M17" s="4">
+      <c r="N17" s="4">
         <v>4.6500000000000004</v>
       </c>
-      <c r="N17" s="2">
+      <c r="O17" s="2">
         <f t="shared" si="1"/>
         <v>91.63000000000001</v>
       </c>
-      <c r="O17" s="3">
+      <c r="P17" s="3">
         <f t="shared" si="2"/>
         <v>3.883</v>
       </c>
-      <c r="P17" s="3">
+      <c r="Q17" s="3">
         <f t="shared" si="3"/>
         <v>132.15400000000002</v>
       </c>
-      <c r="Q17" s="3">
+      <c r="R17" s="3">
         <f t="shared" si="4"/>
         <v>46.288000000000004</v>
       </c>
-      <c r="R17" s="4">
+      <c r="S17" s="4">
         <f t="shared" si="5"/>
         <v>5.1150000000000011</v>
       </c>
-      <c r="S17" s="2">
+      <c r="T17" s="2">
         <f t="shared" si="6"/>
         <v>79.134999999999991</v>
       </c>
-      <c r="T17" s="2">
+      <c r="U17" s="2">
         <f t="shared" si="7"/>
         <v>3.3534999999999995</v>
       </c>
-      <c r="U17" s="2">
+      <c r="V17" s="2">
         <f t="shared" si="8"/>
         <v>114.133</v>
       </c>
-      <c r="V17" s="2">
+      <c r="W17" s="2">
         <f t="shared" si="9"/>
         <v>39.975999999999999</v>
       </c>
-      <c r="W17" s="2">
+      <c r="X17" s="2">
         <f t="shared" si="10"/>
         <v>4.4175000000000004</v>
       </c>
     </row>
-    <row r="18" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
         <v>14</v>
       </c>
@@ -1913,69 +1961,72 @@
         <v>-101.81062300000001</v>
       </c>
       <c r="G18" s="1">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="H18" s="1">
         <v>905.5</v>
       </c>
-      <c r="H18" s="8">
+      <c r="I18" s="8">
         <f t="shared" si="11"/>
         <v>1.2090871001382097</v>
       </c>
-      <c r="I18" s="2">
+      <c r="J18" s="2">
         <v>6.08</v>
       </c>
-      <c r="J18" s="3">
+      <c r="K18" s="3">
         <v>0.42</v>
       </c>
-      <c r="K18" s="3">
+      <c r="L18" s="3">
         <v>15.43</v>
       </c>
-      <c r="L18" s="3">
+      <c r="M18" s="3">
         <v>5.68</v>
       </c>
-      <c r="M18" s="4">
+      <c r="N18" s="4">
         <v>2.0699999999999998</v>
       </c>
-      <c r="N18" s="2">
+      <c r="O18" s="2">
         <f t="shared" si="1"/>
         <v>6.6880000000000006</v>
       </c>
-      <c r="O18" s="3">
+      <c r="P18" s="3">
         <f t="shared" si="2"/>
         <v>0.46200000000000002</v>
       </c>
-      <c r="P18" s="3">
+      <c r="Q18" s="3">
         <f t="shared" si="3"/>
         <v>16.973000000000003</v>
       </c>
-      <c r="Q18" s="3">
+      <c r="R18" s="3">
         <f t="shared" si="4"/>
         <v>6.2480000000000002</v>
       </c>
-      <c r="R18" s="4">
+      <c r="S18" s="4">
         <f t="shared" si="5"/>
         <v>2.2770000000000001</v>
       </c>
-      <c r="S18" s="2">
+      <c r="T18" s="2">
         <f t="shared" si="6"/>
         <v>5.7759999999999998</v>
       </c>
-      <c r="T18" s="2">
+      <c r="U18" s="2">
         <f t="shared" si="7"/>
         <v>0.39899999999999997</v>
       </c>
-      <c r="U18" s="2">
+      <c r="V18" s="2">
         <f t="shared" si="8"/>
         <v>14.658499999999998</v>
       </c>
-      <c r="V18" s="2">
+      <c r="W18" s="2">
         <f t="shared" si="9"/>
         <v>5.3959999999999999</v>
       </c>
-      <c r="W18" s="2">
+      <c r="X18" s="2">
         <f t="shared" si="10"/>
         <v>1.9664999999999997</v>
       </c>
     </row>
-    <row r="19" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
         <v>15</v>
       </c>
@@ -1995,69 +2046,72 @@
         <v>-102.07405900000001</v>
       </c>
       <c r="G19" s="1">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="H19" s="1">
         <v>996.3</v>
       </c>
-      <c r="H19" s="8">
+      <c r="I19" s="8">
         <f t="shared" si="11"/>
         <v>1.1985951953533427</v>
       </c>
-      <c r="I19" s="2">
+      <c r="J19" s="2">
         <v>6.04</v>
       </c>
-      <c r="J19" s="3">
+      <c r="K19" s="3">
         <v>0.86</v>
       </c>
-      <c r="K19" s="3">
+      <c r="L19" s="3">
         <v>9.3699999999999992</v>
       </c>
-      <c r="L19" s="3">
+      <c r="M19" s="3">
         <v>13.38</v>
       </c>
-      <c r="M19" s="4">
+      <c r="N19" s="4">
         <v>1.74</v>
       </c>
-      <c r="N19" s="2">
+      <c r="O19" s="2">
         <f t="shared" si="1"/>
         <v>6.644000000000001</v>
       </c>
-      <c r="O19" s="3">
+      <c r="P19" s="3">
         <f t="shared" si="2"/>
         <v>0.94600000000000006</v>
       </c>
-      <c r="P19" s="3">
+      <c r="Q19" s="3">
         <f t="shared" si="3"/>
         <v>10.307</v>
       </c>
-      <c r="Q19" s="3">
+      <c r="R19" s="3">
         <f t="shared" si="4"/>
         <v>14.718000000000002</v>
       </c>
-      <c r="R19" s="4">
+      <c r="S19" s="4">
         <f t="shared" si="5"/>
         <v>1.9140000000000001</v>
       </c>
-      <c r="S19" s="2">
+      <c r="T19" s="2">
         <f t="shared" si="6"/>
         <v>5.7379999999999995</v>
       </c>
-      <c r="T19" s="2">
+      <c r="U19" s="2">
         <f t="shared" si="7"/>
         <v>0.81699999999999995</v>
       </c>
-      <c r="U19" s="2">
+      <c r="V19" s="2">
         <f t="shared" si="8"/>
         <v>8.9014999999999986</v>
       </c>
-      <c r="V19" s="2">
+      <c r="W19" s="2">
         <f t="shared" si="9"/>
         <v>12.711</v>
       </c>
-      <c r="W19" s="2">
+      <c r="X19" s="2">
         <f t="shared" si="10"/>
         <v>1.653</v>
       </c>
     </row>
-    <row r="20" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
         <v>16</v>
       </c>
@@ -2077,69 +2131,72 @@
         <v>-99.818849999999998</v>
       </c>
       <c r="G20" s="1">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="H20" s="1">
         <v>666.9</v>
       </c>
-      <c r="H20" s="8">
+      <c r="I20" s="8">
         <f t="shared" si="11"/>
         <v>2.0971117481552666</v>
       </c>
-      <c r="I20" s="2">
+      <c r="J20" s="2">
         <v>10.63</v>
       </c>
-      <c r="J20" s="3">
+      <c r="K20" s="3">
         <v>0.89</v>
       </c>
-      <c r="K20" s="3">
+      <c r="L20" s="3">
         <v>20.18</v>
       </c>
-      <c r="L20" s="3">
+      <c r="M20" s="3">
         <v>11.01</v>
       </c>
-      <c r="M20" s="4">
+      <c r="N20" s="4">
         <v>1.85</v>
       </c>
-      <c r="N20" s="2">
+      <c r="O20" s="2">
         <f t="shared" si="1"/>
         <v>11.693000000000001</v>
       </c>
-      <c r="O20" s="3">
+      <c r="P20" s="3">
         <f t="shared" si="2"/>
         <v>0.97900000000000009</v>
       </c>
-      <c r="P20" s="3">
+      <c r="Q20" s="3">
         <f t="shared" si="3"/>
         <v>22.198</v>
       </c>
-      <c r="Q20" s="3">
+      <c r="R20" s="3">
         <f t="shared" si="4"/>
         <v>12.111000000000001</v>
       </c>
-      <c r="R20" s="4">
+      <c r="S20" s="4">
         <f t="shared" si="5"/>
         <v>2.0350000000000001</v>
       </c>
-      <c r="S20" s="2">
+      <c r="T20" s="2">
         <f t="shared" si="6"/>
         <v>10.0985</v>
       </c>
-      <c r="T20" s="2">
+      <c r="U20" s="2">
         <f t="shared" si="7"/>
         <v>0.84549999999999992</v>
       </c>
-      <c r="U20" s="2">
+      <c r="V20" s="2">
         <f t="shared" si="8"/>
         <v>19.170999999999999</v>
       </c>
-      <c r="V20" s="2">
+      <c r="W20" s="2">
         <f t="shared" si="9"/>
         <v>10.459499999999998</v>
       </c>
-      <c r="W20" s="2">
+      <c r="X20" s="2">
         <f t="shared" si="10"/>
         <v>1.7575000000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
         <v>17</v>
       </c>
@@ -2159,73 +2216,76 @@
         <v>-96.901972999999998</v>
       </c>
       <c r="G21" s="1">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="H21" s="1">
         <v>594</v>
       </c>
-      <c r="H21" s="8">
+      <c r="I21" s="8">
         <f t="shared" si="11"/>
         <v>1.6999910326326615</v>
       </c>
-      <c r="I21" s="5">
+      <c r="J21" s="5">
         <v>8.2799999999999994</v>
       </c>
-      <c r="J21" s="6">
+      <c r="K21" s="6">
         <v>1.5</v>
       </c>
-      <c r="K21" s="6">
+      <c r="L21" s="6">
         <v>16.22</v>
       </c>
-      <c r="L21" s="6">
+      <c r="M21" s="6">
         <v>13.69</v>
       </c>
-      <c r="M21" s="7">
+      <c r="N21" s="7">
         <v>5.55</v>
       </c>
-      <c r="N21" s="2">
+      <c r="O21" s="2">
         <f t="shared" si="1"/>
         <v>9.1080000000000005</v>
       </c>
-      <c r="O21" s="3">
+      <c r="P21" s="3">
         <f t="shared" si="2"/>
         <v>1.6500000000000001</v>
       </c>
-      <c r="P21" s="3">
+      <c r="Q21" s="3">
         <f t="shared" si="3"/>
         <v>17.841999999999999</v>
       </c>
-      <c r="Q21" s="3">
+      <c r="R21" s="3">
         <f t="shared" si="4"/>
         <v>15.059000000000001</v>
       </c>
-      <c r="R21" s="4">
+      <c r="S21" s="4">
         <f t="shared" si="5"/>
         <v>6.1050000000000004</v>
       </c>
-      <c r="S21" s="2">
+      <c r="T21" s="2">
         <f t="shared" si="6"/>
         <v>7.8659999999999988</v>
       </c>
-      <c r="T21" s="2">
+      <c r="U21" s="2">
         <f t="shared" si="7"/>
         <v>1.4249999999999998</v>
       </c>
-      <c r="U21" s="2">
+      <c r="V21" s="2">
         <f t="shared" si="8"/>
         <v>15.408999999999999</v>
       </c>
-      <c r="V21" s="2">
+      <c r="W21" s="2">
         <f t="shared" si="9"/>
         <v>13.0055</v>
       </c>
-      <c r="W21" s="2">
+      <c r="X21" s="2">
         <f t="shared" si="10"/>
         <v>5.2725</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="I2:M2"/>
-    <mergeCell ref="N2:R2"/>
-    <mergeCell ref="S2:W2"/>
+    <mergeCell ref="J2:N2"/>
+    <mergeCell ref="O2:S2"/>
+    <mergeCell ref="T2:X2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B19" r:id="rId1" tooltip="Michoacán" display="https://en.wikipedia.org/wiki/Michoac%C3%A1n" xr:uid="{00000000-0004-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
Intermediate commit to rebase some stuff...
</commit_message>
<xml_diff>
--- a/tests/data/complete_pgm.xlsx
+++ b/tests/data/complete_pgm.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10319"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mhearne/src/python/shakemap-amp-tools/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{E8DDEBD0-A1ED-1841-9F05-AFA218E421AD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C280D847-FD8C-A745-AFDF-90475A982D59}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="460" windowWidth="26200" windowHeight="13700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="spectral_values.csv" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="49">
   <si>
     <t>ACAM</t>
   </si>
@@ -79,21 +79,6 @@
     <t>station</t>
   </si>
   <si>
-    <t>pga</t>
-  </si>
-  <si>
-    <t>pgv</t>
-  </si>
-  <si>
-    <t>psa03</t>
-  </si>
-  <si>
-    <t>psa10</t>
-  </si>
-  <si>
-    <t>psa30</t>
-  </si>
-  <si>
     <t>intensity</t>
   </si>
   <si>
@@ -164,6 +149,24 @@
   </si>
   <si>
     <t>elev</t>
+  </si>
+  <si>
+    <t>PGA</t>
+  </si>
+  <si>
+    <t>PGV</t>
+  </si>
+  <si>
+    <t>SA(0.3)</t>
+  </si>
+  <si>
+    <t>SA(1.0)</t>
+  </si>
+  <si>
+    <t>SA(3.0)</t>
+  </si>
+  <si>
+    <t>SA(0.3_</t>
   </si>
 </sst>
 </file>
@@ -627,8 +630,8 @@
   </sheetPr>
   <dimension ref="A1:X21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -650,10 +653,10 @@
   <sheetData>
     <row r="1" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -661,45 +664,45 @@
         <v>18</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="G2" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="K2" s="11"/>
       <c r="L2" s="11"/>
       <c r="M2" s="11"/>
       <c r="N2" s="12"/>
       <c r="O2" s="10" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="P2" s="11"/>
       <c r="Q2" s="11"/>
       <c r="R2" s="11"/>
       <c r="S2" s="12"/>
       <c r="T2" s="10" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="U2" s="11"/>
       <c r="V2" s="11"/>
@@ -708,49 +711,49 @@
     </row>
     <row r="3" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="J3" s="2" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="R3" s="3" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
       <c r="S3" s="4" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="U3" s="3" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="V3" s="3" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="W3" s="3" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
       <c r="X3" s="4" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -758,13 +761,13 @@
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E4" s="1">
         <v>20.043185999999999</v>
@@ -843,13 +846,13 @@
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E5" s="1">
         <v>16.874293999999999</v>
@@ -928,13 +931,13 @@
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E6" s="1">
         <v>17.213360999999999</v>
@@ -1013,13 +1016,13 @@
         <v>3</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E7" s="1">
         <v>16.247374000000001</v>
@@ -1097,13 +1100,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E8" s="1">
         <v>19.325265999999999</v>
@@ -1181,13 +1184,13 @@
         <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E9" s="1">
         <v>16.997788</v>
@@ -1266,13 +1269,13 @@
         <v>6</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E10" s="1">
         <v>17.798341000000001</v>
@@ -1351,13 +1354,13 @@
         <v>7</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E11" s="1">
         <v>16.565152999999999</v>
@@ -1436,13 +1439,13 @@
         <v>8</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E12" s="1">
         <v>17.067336999999998</v>
@@ -1521,13 +1524,13 @@
         <v>9</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E13" s="1">
         <v>17.065038999999999</v>
@@ -1606,13 +1609,13 @@
         <v>10</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E14" s="1">
         <v>15.666836999999999</v>
@@ -1691,13 +1694,13 @@
         <v>11</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E15" s="1">
         <v>17.535395999999999</v>
@@ -1776,13 +1779,13 @@
         <v>12</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="E16" s="1">
         <v>19.044222999999999</v>
@@ -1861,13 +1864,13 @@
         <v>13</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E17" s="1">
         <v>18.904050999999999</v>
@@ -1946,13 +1949,13 @@
         <v>14</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E18" s="1">
         <v>17.98762</v>
@@ -2031,13 +2034,13 @@
         <v>15</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E19" s="1">
         <v>19.421758000000001</v>
@@ -2116,13 +2119,13 @@
         <v>16</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E20" s="1">
         <v>16.914259999999999</v>
@@ -2201,13 +2204,13 @@
         <v>17</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E21" s="1">
         <v>19.529875000000001</v>

</xml_diff>

<commit_message>
spreadsheet column names now must all be upper case, channel names are all now H1,H2 instead of HHE,HHN.
</commit_message>
<xml_diff>
--- a/tests/data/complete_pgm.xlsx
+++ b/tests/data/complete_pgm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mhearne/src/python/shakemap-amp-tools/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C280D847-FD8C-A745-AFDF-90475A982D59}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA731DDD-CF88-ED43-886D-65087A8C9625}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="460" windowWidth="26200" windowHeight="13700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -79,9 +79,6 @@
     <t>station</t>
   </si>
   <si>
-    <t>intensity</t>
-  </si>
-  <si>
     <t>MX</t>
   </si>
   <si>
@@ -94,9 +91,6 @@
     <t>Z</t>
   </si>
   <si>
-    <t>distance</t>
-  </si>
-  <si>
     <t>Guanajuato</t>
   </si>
   <si>
@@ -124,9 +118,6 @@
     <t>Veracruz</t>
   </si>
   <si>
-    <t>source</t>
-  </si>
-  <si>
     <t>National Seismic Service</t>
   </si>
   <si>
@@ -136,21 +127,6 @@
     <t>Mexican National Seismic Service report dated 2010-01-01</t>
   </si>
   <si>
-    <t>lat</t>
-  </si>
-  <si>
-    <t>lon</t>
-  </si>
-  <si>
-    <t>netid</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>elev</t>
-  </si>
-  <si>
     <t>PGA</t>
   </si>
   <si>
@@ -167,6 +143,30 @@
   </si>
   <si>
     <t>SA(0.3_</t>
+  </si>
+  <si>
+    <t>NAME</t>
+  </si>
+  <si>
+    <t>NETID</t>
+  </si>
+  <si>
+    <t>SOURCE</t>
+  </si>
+  <si>
+    <t>LAT</t>
+  </si>
+  <si>
+    <t>LON</t>
+  </si>
+  <si>
+    <t>ELEV</t>
+  </si>
+  <si>
+    <t>DISTANCE</t>
+  </si>
+  <si>
+    <t>INTENSITY</t>
   </si>
 </sst>
 </file>
@@ -631,12 +631,12 @@
   <dimension ref="A1:X21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="9" max="9" width="7.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10" style="9" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7.1640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="5.1640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="7.1640625" bestFit="1" customWidth="1"/>
@@ -653,10 +653,10 @@
   <sheetData>
     <row r="1" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -667,42 +667,42 @@
         <v>41</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>24</v>
+        <v>47</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K2" s="11"/>
       <c r="L2" s="11"/>
       <c r="M2" s="11"/>
       <c r="N2" s="12"/>
       <c r="O2" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="P2" s="11"/>
       <c r="Q2" s="11"/>
       <c r="R2" s="11"/>
       <c r="S2" s="12"/>
       <c r="T2" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="U2" s="11"/>
       <c r="V2" s="11"/>
@@ -711,49 +711,49 @@
     </row>
     <row r="3" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="J3" s="2" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="R3" s="3" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="S3" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="U3" s="3" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="V3" s="3" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="W3" s="3" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="X3" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -761,13 +761,13 @@
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E4" s="1">
         <v>20.043185999999999</v>
@@ -846,13 +846,13 @@
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E5" s="1">
         <v>16.874293999999999</v>
@@ -931,13 +931,13 @@
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E6" s="1">
         <v>17.213360999999999</v>
@@ -1016,13 +1016,13 @@
         <v>3</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E7" s="1">
         <v>16.247374000000001</v>
@@ -1100,13 +1100,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E8" s="1">
         <v>19.325265999999999</v>
@@ -1184,13 +1184,13 @@
         <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E9" s="1">
         <v>16.997788</v>
@@ -1269,13 +1269,13 @@
         <v>6</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E10" s="1">
         <v>17.798341000000001</v>
@@ -1354,13 +1354,13 @@
         <v>7</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E11" s="1">
         <v>16.565152999999999</v>
@@ -1439,13 +1439,13 @@
         <v>8</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E12" s="1">
         <v>17.067336999999998</v>
@@ -1524,13 +1524,13 @@
         <v>9</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E13" s="1">
         <v>17.065038999999999</v>
@@ -1609,13 +1609,13 @@
         <v>10</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E14" s="1">
         <v>15.666836999999999</v>
@@ -1694,13 +1694,13 @@
         <v>11</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E15" s="1">
         <v>17.535395999999999</v>
@@ -1779,13 +1779,13 @@
         <v>12</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E16" s="1">
         <v>19.044222999999999</v>
@@ -1864,13 +1864,13 @@
         <v>13</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E17" s="1">
         <v>18.904050999999999</v>
@@ -1949,13 +1949,13 @@
         <v>14</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E18" s="1">
         <v>17.98762</v>
@@ -2034,13 +2034,13 @@
         <v>15</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="E19" s="1">
         <v>19.421758000000001</v>
@@ -2119,13 +2119,13 @@
         <v>16</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E20" s="1">
         <v>16.914259999999999</v>
@@ -2204,13 +2204,13 @@
         <v>17</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E21" s="1">
         <v>19.529875000000001</v>

</xml_diff>